<commit_message>
recommender update, add rID and distance
</commit_message>
<xml_diff>
--- a/mySQL/爬蟲/crawler.xlsx
+++ b/mySQL/爬蟲/crawler.xlsx
@@ -2712,1036 +2712,2278 @@
       <c r="A208" t="n">
         <v>223</v>
       </c>
+      <c r="B208" t="n">
+        <v>23.963696</v>
+      </c>
+      <c r="C208" t="n">
+        <v>120.9632693753426</v>
+      </c>
     </row>
     <row r="209">
       <c r="A209" t="n">
         <v>224</v>
       </c>
+      <c r="B209" t="n">
+        <v>23.96791</v>
+      </c>
+      <c r="C209" t="n">
+        <v>120.9715010753426</v>
+      </c>
     </row>
     <row r="210">
       <c r="A210" t="n">
         <v>225</v>
       </c>
+      <c r="B210" t="n">
+        <v>23.965289</v>
+      </c>
+      <c r="C210" t="n">
+        <v>120.9645762753425</v>
+      </c>
     </row>
     <row r="211">
       <c r="A211" t="n">
         <v>227</v>
       </c>
+      <c r="B211" t="n">
+        <v>23.96423</v>
+      </c>
+      <c r="C211" t="n">
+        <v>120.9612292753425</v>
+      </c>
     </row>
     <row r="212">
       <c r="A212" t="n">
         <v>228</v>
       </c>
+      <c r="B212" t="n">
+        <v>23.959758</v>
+      </c>
+      <c r="C212" t="n">
+        <v>120.9611155753424</v>
+      </c>
     </row>
     <row r="213">
       <c r="A213" t="n">
         <v>229</v>
       </c>
+      <c r="B213" t="n">
+        <v>23.967996</v>
+      </c>
+      <c r="C213" t="n">
+        <v>120.9499988753425</v>
+      </c>
     </row>
     <row r="214">
       <c r="A214" t="n">
         <v>230</v>
       </c>
+      <c r="B214" t="n">
+        <v>23.97138</v>
+      </c>
+      <c r="C214" t="n">
+        <v>120.9664817753428</v>
+      </c>
     </row>
     <row r="215">
       <c r="A215" t="n">
         <v>231</v>
       </c>
+      <c r="B215" t="n">
+        <v>23.962908</v>
+      </c>
+      <c r="C215" t="n">
+        <v>120.9605757753426</v>
+      </c>
     </row>
     <row r="216">
       <c r="A216" t="n">
         <v>232</v>
       </c>
+      <c r="B216" t="n">
+        <v>23.965883</v>
+      </c>
+      <c r="C216" t="n">
+        <v>120.9652869753425</v>
+      </c>
     </row>
     <row r="217">
       <c r="A217" t="n">
         <v>233</v>
       </c>
+      <c r="B217" t="n">
+        <v>23.947588</v>
+      </c>
+      <c r="C217" t="n">
+        <v>120.9199492216908</v>
+      </c>
     </row>
     <row r="218">
       <c r="A218" t="n">
         <v>234</v>
       </c>
+      <c r="B218" t="n">
+        <v>23.96105</v>
+      </c>
+      <c r="C218" t="n">
+        <v>120.9691721753425</v>
+      </c>
     </row>
     <row r="219">
       <c r="A219" t="n">
         <v>235</v>
       </c>
+      <c r="B219" t="n">
+        <v>23.967215</v>
+      </c>
+      <c r="C219" t="n">
+        <v>120.9650603753427</v>
+      </c>
     </row>
     <row r="220">
       <c r="A220" t="n">
         <v>236</v>
       </c>
+      <c r="B220" t="n">
+        <v>23.957604</v>
+      </c>
+      <c r="C220" t="n">
+        <v>120.9723904753424</v>
+      </c>
     </row>
     <row r="221">
       <c r="A221" t="n">
         <v>237</v>
       </c>
+      <c r="B221" t="n">
+        <v>23.971571</v>
+      </c>
+      <c r="C221" t="n">
+        <v>120.9599631753428</v>
+      </c>
     </row>
     <row r="222">
       <c r="A222" t="n">
         <v>238</v>
       </c>
+      <c r="B222" t="n">
+        <v>23.969772</v>
+      </c>
+      <c r="C222" t="n">
+        <v>120.9504691753429</v>
+      </c>
     </row>
     <row r="223">
       <c r="A223" t="n">
         <v>239</v>
       </c>
+      <c r="B223" t="n">
+        <v>23.9668</v>
+      </c>
+      <c r="C223" t="n">
+        <v>120.9693096753426</v>
+      </c>
     </row>
     <row r="224">
       <c r="A224" t="n">
         <v>241</v>
       </c>
+      <c r="B224" t="n">
+        <v>23.96578</v>
+      </c>
+      <c r="C224" t="n">
+        <v>120.9638065753426</v>
+      </c>
     </row>
     <row r="225">
       <c r="A225" t="n">
         <v>242</v>
       </c>
+      <c r="B225" t="n">
+        <v>23.97457</v>
+      </c>
+      <c r="C225" t="n">
+        <v>120.9402343753428</v>
+      </c>
     </row>
     <row r="226">
       <c r="A226" t="n">
         <v>243</v>
       </c>
+      <c r="B226" t="n">
+        <v>23.96312</v>
+      </c>
+      <c r="C226" t="n">
+        <v>120.9604041753425</v>
+      </c>
     </row>
     <row r="227">
       <c r="A227" t="n">
         <v>244</v>
       </c>
+      <c r="B227" t="n">
+        <v>23.97213</v>
+      </c>
+      <c r="C227" t="n">
+        <v>120.9748272753428</v>
+      </c>
     </row>
     <row r="228">
       <c r="A228" t="n">
         <v>245</v>
       </c>
+      <c r="B228" t="n">
+        <v>23.963664</v>
+      </c>
+      <c r="C228" t="n">
+        <v>120.9616464753426</v>
+      </c>
     </row>
     <row r="229">
       <c r="A229" t="n">
         <v>246</v>
       </c>
+      <c r="B229" t="n">
+        <v>23.97694237</v>
+      </c>
+      <c r="C229" t="n">
+        <v>120.985563175343</v>
+      </c>
     </row>
     <row r="230">
       <c r="A230" t="n">
         <v>247</v>
       </c>
+      <c r="B230" t="n">
+        <v>23.96938</v>
+      </c>
+      <c r="C230" t="n">
+        <v>120.9666626753427</v>
+      </c>
     </row>
     <row r="231">
       <c r="A231" t="n">
         <v>248</v>
       </c>
+      <c r="B231" t="n">
+        <v>23.96094</v>
+      </c>
+      <c r="C231" t="n">
+        <v>120.9562365753425</v>
+      </c>
     </row>
     <row r="232">
       <c r="A232" t="n">
         <v>249</v>
       </c>
+      <c r="B232" t="n">
+        <v>23.972364</v>
+      </c>
+      <c r="C232" t="n">
+        <v>120.9648702753427</v>
+      </c>
     </row>
     <row r="233">
       <c r="A233" t="n">
         <v>250</v>
       </c>
+      <c r="B233" t="n">
+        <v>23.968746</v>
+      </c>
+      <c r="C233" t="n">
+        <v>120.9688910753427</v>
+      </c>
     </row>
     <row r="234">
       <c r="A234" t="n">
         <v>251</v>
       </c>
+      <c r="B234" t="n">
+        <v>23.95998</v>
+      </c>
+      <c r="C234" t="n">
+        <v>120.9602897753424</v>
+      </c>
     </row>
     <row r="235">
       <c r="A235" t="n">
         <v>252</v>
       </c>
+      <c r="B235" t="n">
+        <v>23.970525</v>
+      </c>
+      <c r="C235" t="n">
+        <v>120.9653918753427</v>
+      </c>
     </row>
     <row r="236">
       <c r="A236" t="n">
         <v>253</v>
       </c>
+      <c r="B236" t="n">
+        <v>23.968036</v>
+      </c>
+      <c r="C236" t="n">
+        <v>120.9663322753426</v>
+      </c>
     </row>
     <row r="237">
       <c r="A237" t="n">
         <v>254</v>
       </c>
+      <c r="B237" t="n">
+        <v>24.006267</v>
+      </c>
+      <c r="C237" t="n">
+        <v>120.9522720753439</v>
+      </c>
     </row>
     <row r="238">
       <c r="A238" t="n">
         <v>255</v>
       </c>
+      <c r="B238" t="n">
+        <v>23.96252</v>
+      </c>
+      <c r="C238" t="n">
+        <v>120.9638010753425</v>
+      </c>
     </row>
     <row r="239">
       <c r="A239" t="n">
         <v>256</v>
       </c>
+      <c r="B239" t="n">
+        <v>23.9609</v>
+      </c>
+      <c r="C239" t="n">
+        <v>120.9649788753424</v>
+      </c>
     </row>
     <row r="240">
       <c r="A240" t="n">
         <v>257</v>
       </c>
+      <c r="B240" t="n">
+        <v>23.97133</v>
+      </c>
+      <c r="C240" t="n">
+        <v>120.9622502753428</v>
+      </c>
     </row>
     <row r="241">
       <c r="A241" t="n">
         <v>260</v>
       </c>
+      <c r="B241" t="n">
+        <v>23.97021</v>
+      </c>
+      <c r="C241" t="n">
+        <v>120.9703523753428</v>
+      </c>
     </row>
     <row r="242">
       <c r="A242" t="n">
         <v>261</v>
       </c>
+      <c r="B242" t="n">
+        <v>23.96549</v>
+      </c>
+      <c r="C242" t="n">
+        <v>120.9661073753425</v>
+      </c>
     </row>
     <row r="243">
       <c r="A243" t="n">
         <v>263</v>
       </c>
+      <c r="B243" t="n">
+        <v>23.947588</v>
+      </c>
+      <c r="C243" t="n">
+        <v>120.9199492216908</v>
+      </c>
     </row>
     <row r="244">
       <c r="A244" t="n">
         <v>264</v>
       </c>
+      <c r="B244" t="n">
+        <v>23.9676119</v>
+      </c>
+      <c r="C244" t="n">
+        <v>120.9672150753427</v>
+      </c>
     </row>
     <row r="245">
       <c r="A245" t="n">
         <v>265</v>
       </c>
+      <c r="B245" t="n">
+        <v>23.963458</v>
+      </c>
+      <c r="C245" t="n">
+        <v>120.9663637753425</v>
+      </c>
     </row>
     <row r="246">
       <c r="A246" t="n">
         <v>266</v>
       </c>
+      <c r="B246" t="n">
+        <v>23.97289</v>
+      </c>
+      <c r="C246" t="n">
+        <v>120.9611644753429</v>
+      </c>
     </row>
     <row r="247">
       <c r="A247" t="n">
         <v>267</v>
       </c>
+      <c r="B247" t="n">
+        <v>23.96475</v>
+      </c>
+      <c r="C247" t="n">
+        <v>120.9660777753426</v>
+      </c>
     </row>
     <row r="248">
       <c r="A248" t="n">
         <v>269</v>
       </c>
+      <c r="B248" t="n">
+        <v>23.96668</v>
+      </c>
+      <c r="C248" t="n">
+        <v>120.9647764753427</v>
+      </c>
     </row>
     <row r="249">
       <c r="A249" t="n">
         <v>270</v>
       </c>
+      <c r="B249" t="n">
+        <v>23.965663</v>
+      </c>
+      <c r="C249" t="n">
+        <v>120.9656167753426</v>
+      </c>
     </row>
     <row r="250">
       <c r="A250" t="n">
         <v>271</v>
       </c>
+      <c r="B250" t="n">
+        <v>23.96796597</v>
+      </c>
+      <c r="C250" t="n">
+        <v>120.9676699753427</v>
+      </c>
     </row>
     <row r="251">
       <c r="A251" t="n">
         <v>272</v>
       </c>
+      <c r="B251" t="n">
+        <v>23.970589</v>
+      </c>
+      <c r="C251" t="n">
+        <v>120.9536652753429</v>
+      </c>
     </row>
     <row r="252">
       <c r="A252" t="n">
         <v>273</v>
       </c>
+      <c r="B252" t="n">
+        <v>23.9896987</v>
+      </c>
+      <c r="C252" t="n">
+        <v>120.9718802753433</v>
+      </c>
     </row>
     <row r="253">
       <c r="A253" t="n">
         <v>274</v>
       </c>
+      <c r="B253" t="n">
+        <v>23.9734</v>
+      </c>
+      <c r="C253" t="n">
+        <v>120.9672350753428</v>
+      </c>
     </row>
     <row r="254">
       <c r="A254" t="n">
         <v>275</v>
       </c>
+      <c r="B254" t="n">
+        <v>23.96585</v>
+      </c>
+      <c r="C254" t="n">
+        <v>120.9703694753426</v>
+      </c>
     </row>
     <row r="255">
       <c r="A255" t="n">
         <v>276</v>
       </c>
+      <c r="B255" t="n">
+        <v>23.96712</v>
+      </c>
+      <c r="C255" t="n">
+        <v>120.9654891753425</v>
+      </c>
     </row>
     <row r="256">
       <c r="A256" t="n">
         <v>277</v>
       </c>
+      <c r="B256" t="n">
+        <v>23.96983</v>
+      </c>
+      <c r="C256" t="n">
+        <v>120.9750483753427</v>
+      </c>
     </row>
     <row r="257">
       <c r="A257" t="n">
         <v>278</v>
       </c>
+      <c r="B257" t="n">
+        <v>23.959915</v>
+      </c>
+      <c r="C257" t="n">
+        <v>120.9653996753425</v>
+      </c>
     </row>
     <row r="258">
       <c r="A258" t="n">
         <v>279</v>
       </c>
+      <c r="B258" t="n">
+        <v>23.964295</v>
+      </c>
+      <c r="C258" t="n">
+        <v>120.9620496753425</v>
+      </c>
     </row>
     <row r="259">
       <c r="A259" t="n">
         <v>280</v>
       </c>
+      <c r="B259" t="n">
+        <v>23.971073</v>
+      </c>
+      <c r="C259" t="n">
+        <v>120.9551073033143</v>
+      </c>
     </row>
     <row r="260">
       <c r="A260" t="n">
         <v>281</v>
       </c>
+      <c r="B260" t="n">
+        <v>23.978936</v>
+      </c>
+      <c r="C260" t="n">
+        <v>120.8091339670266</v>
+      </c>
     </row>
     <row r="261">
       <c r="A261" t="n">
         <v>282</v>
       </c>
+      <c r="B261" t="n">
+        <v>23.970586</v>
+      </c>
+      <c r="C261" t="n">
+        <v>120.9640274753428</v>
+      </c>
     </row>
     <row r="262">
       <c r="A262" t="n">
         <v>283</v>
       </c>
+      <c r="B262" t="n">
+        <v>23.96529</v>
+      </c>
+      <c r="C262" t="n">
+        <v>120.9677984753426</v>
+      </c>
     </row>
     <row r="263">
       <c r="A263" t="n">
         <v>284</v>
       </c>
+      <c r="B263" t="n">
+        <v>23.96831</v>
+      </c>
+      <c r="C263" t="n">
+        <v>120.9688150753427</v>
+      </c>
     </row>
     <row r="264">
       <c r="A264" t="n">
         <v>286</v>
       </c>
+      <c r="B264" t="n">
+        <v>23.96694</v>
+      </c>
+      <c r="C264" t="n">
+        <v>120.9631200753425</v>
+      </c>
     </row>
     <row r="265">
       <c r="A265" t="n">
         <v>287</v>
       </c>
+      <c r="B265" t="n">
+        <v>23.96752</v>
+      </c>
+      <c r="C265" t="n">
+        <v>120.9671134753426</v>
+      </c>
     </row>
     <row r="266">
       <c r="A266" t="n">
         <v>288</v>
       </c>
+      <c r="B266" t="n">
+        <v>23.962723</v>
+      </c>
+      <c r="C266" t="n">
+        <v>120.9603433753426</v>
+      </c>
     </row>
     <row r="267">
       <c r="A267" t="n">
         <v>289</v>
       </c>
+      <c r="B267" t="n">
+        <v>23.968365</v>
+      </c>
+      <c r="C267" t="n">
+        <v>120.9689132753428</v>
+      </c>
     </row>
     <row r="268">
       <c r="A268" t="n">
         <v>290</v>
       </c>
+      <c r="B268" t="n">
+        <v>23.96381</v>
+      </c>
+      <c r="C268" t="n">
+        <v>120.9630486753425</v>
+      </c>
     </row>
     <row r="269">
       <c r="A269" t="n">
         <v>291</v>
       </c>
+      <c r="B269" t="n">
+        <v>23.96189</v>
+      </c>
+      <c r="C269" t="n">
+        <v>120.9670474753426</v>
+      </c>
     </row>
     <row r="270">
       <c r="A270" t="n">
         <v>292</v>
       </c>
+      <c r="B270" t="n">
+        <v>23.96689</v>
+      </c>
+      <c r="C270" t="n">
+        <v>120.9649118753427</v>
+      </c>
     </row>
     <row r="271">
       <c r="A271" t="n">
         <v>293</v>
       </c>
+      <c r="B271" t="n">
+        <v>23.95939</v>
+      </c>
+      <c r="C271" t="n">
+        <v>120.9617358753424</v>
+      </c>
     </row>
     <row r="272">
       <c r="A272" t="n">
         <v>294</v>
       </c>
+      <c r="B272" t="n">
+        <v>23.96761</v>
+      </c>
+      <c r="C272" t="n">
+        <v>120.9612152753426</v>
+      </c>
     </row>
     <row r="273">
       <c r="A273" t="n">
         <v>295</v>
       </c>
+      <c r="B273" t="n">
+        <v>23.96664</v>
+      </c>
+      <c r="C273" t="n">
+        <v>120.9681262753426</v>
+      </c>
     </row>
     <row r="274">
       <c r="A274" t="n">
         <v>296</v>
       </c>
+      <c r="B274" t="n">
+        <v>23.972549</v>
+      </c>
+      <c r="C274" t="n">
+        <v>120.9675683753428</v>
+      </c>
     </row>
     <row r="275">
       <c r="A275" t="n">
         <v>297</v>
       </c>
+      <c r="B275" t="n">
+        <v>23.970205</v>
+      </c>
+      <c r="C275" t="n">
+        <v>120.9516174753427</v>
+      </c>
     </row>
     <row r="276">
       <c r="A276" t="n">
         <v>298</v>
       </c>
+      <c r="B276" t="n">
+        <v>23.967381</v>
+      </c>
+      <c r="C276" t="n">
+        <v>120.9675204753427</v>
+      </c>
     </row>
     <row r="277">
       <c r="A277" t="n">
         <v>299</v>
       </c>
+      <c r="B277" t="n">
+        <v>23.973025</v>
+      </c>
+      <c r="C277" t="n">
+        <v>120.9627529753428</v>
+      </c>
     </row>
     <row r="278">
       <c r="A278" t="n">
         <v>300</v>
       </c>
+      <c r="B278" t="n">
+        <v>23.975255</v>
+      </c>
+      <c r="C278" t="n">
+        <v>120.9391143753429</v>
+      </c>
     </row>
     <row r="279">
       <c r="A279" t="n">
         <v>301</v>
       </c>
+      <c r="B279" t="n">
+        <v>23.972467</v>
+      </c>
+      <c r="C279" t="n">
+        <v>120.9671112753427</v>
+      </c>
     </row>
     <row r="280">
       <c r="A280" t="n">
         <v>302</v>
       </c>
+      <c r="B280" t="n">
+        <v>23.9686912</v>
+      </c>
+      <c r="C280" t="n">
+        <v>120.9668972753427</v>
+      </c>
     </row>
     <row r="281">
       <c r="A281" t="n">
         <v>303</v>
       </c>
+      <c r="B281" t="n">
+        <v>23.96673</v>
+      </c>
+      <c r="C281" t="n">
+        <v>120.9643788753426</v>
+      </c>
     </row>
     <row r="282">
       <c r="A282" t="n">
         <v>304</v>
       </c>
+      <c r="B282" t="n">
+        <v>23.967258</v>
+      </c>
+      <c r="C282" t="n">
+        <v>120.9602144753427</v>
+      </c>
     </row>
     <row r="283">
       <c r="A283" t="n">
         <v>305</v>
       </c>
+      <c r="B283" t="n">
+        <v>23.963771</v>
+      </c>
+      <c r="C283" t="n">
+        <v>120.9612098753426</v>
+      </c>
     </row>
     <row r="284">
       <c r="A284" t="n">
         <v>306</v>
       </c>
+      <c r="B284" t="n">
+        <v>23.96298</v>
+      </c>
+      <c r="C284" t="n">
+        <v>120.9281441429879</v>
+      </c>
     </row>
     <row r="285">
       <c r="A285" t="n">
         <v>307</v>
       </c>
+      <c r="B285" t="n">
+        <v>23.96956</v>
+      </c>
+      <c r="C285" t="n">
+        <v>120.9526207753427</v>
+      </c>
     </row>
     <row r="286">
       <c r="A286" t="n">
         <v>309</v>
       </c>
+      <c r="B286" t="n">
+        <v>23.9712</v>
+      </c>
+      <c r="C286" t="n">
+        <v>120.9742713753428</v>
+      </c>
     </row>
     <row r="287">
       <c r="A287" t="n">
         <v>310</v>
       </c>
+      <c r="B287" t="n">
+        <v>23.970004</v>
+      </c>
+      <c r="C287" t="n">
+        <v>120.9659351753428</v>
+      </c>
     </row>
     <row r="288">
       <c r="A288" t="n">
         <v>311</v>
       </c>
+      <c r="B288" t="n">
+        <v>23.962577</v>
+      </c>
+      <c r="C288" t="n">
+        <v>120.9673310753425</v>
+      </c>
     </row>
     <row r="289">
       <c r="A289" t="n">
         <v>312</v>
       </c>
+      <c r="B289" t="n">
+        <v>23.96048</v>
+      </c>
+      <c r="C289" t="n">
+        <v>120.9603784753424</v>
+      </c>
     </row>
     <row r="290">
       <c r="A290" t="n">
         <v>313</v>
       </c>
+      <c r="B290" t="n">
+        <v>23.96158617</v>
+      </c>
+      <c r="C290" t="n">
+        <v>120.9589223753425</v>
+      </c>
     </row>
     <row r="291">
       <c r="A291" t="n">
         <v>314</v>
       </c>
+      <c r="B291" t="n">
+        <v>23.966367</v>
+      </c>
+      <c r="C291" t="n">
+        <v>120.9663597753425</v>
+      </c>
     </row>
     <row r="292">
       <c r="A292" t="n">
         <v>315</v>
       </c>
+      <c r="B292" t="n">
+        <v>23.964273</v>
+      </c>
+      <c r="C292" t="n">
+        <v>120.9617643753426</v>
+      </c>
     </row>
     <row r="293">
       <c r="A293" t="n">
         <v>316</v>
       </c>
+      <c r="B293" t="n">
+        <v>23.95474</v>
+      </c>
+      <c r="C293" t="n">
+        <v>120.9720966753422</v>
+      </c>
     </row>
     <row r="294">
       <c r="A294" t="n">
         <v>317</v>
       </c>
+      <c r="B294" t="n">
+        <v>23.96982</v>
+      </c>
+      <c r="C294" t="n">
+        <v>120.9631105753428</v>
+      </c>
     </row>
     <row r="295">
       <c r="A295" t="n">
         <v>318</v>
       </c>
+      <c r="B295" t="n">
+        <v>23.967442</v>
+      </c>
+      <c r="C295" t="n">
+        <v>120.9675906753425</v>
+      </c>
     </row>
     <row r="296">
       <c r="A296" t="n">
         <v>319</v>
       </c>
+      <c r="B296" t="n">
+        <v>23.97173</v>
+      </c>
+      <c r="C296" t="n">
+        <v>120.9558526753427</v>
+      </c>
     </row>
     <row r="297">
       <c r="A297" t="n">
         <v>320</v>
       </c>
+      <c r="B297" t="n">
+        <v>23.89811</v>
+      </c>
+      <c r="C297" t="n">
+        <v>120.9326338753404</v>
+      </c>
     </row>
     <row r="298">
       <c r="A298" t="n">
         <v>321</v>
       </c>
+      <c r="B298" t="n">
+        <v>23.962997</v>
+      </c>
+      <c r="C298" t="n">
+        <v>120.9662760753425</v>
+      </c>
     </row>
     <row r="299">
       <c r="A299" t="n">
         <v>322</v>
       </c>
+      <c r="B299" t="n">
+        <v>23.97334</v>
+      </c>
+      <c r="C299" t="n">
+        <v>120.9616858753428</v>
+      </c>
     </row>
     <row r="300">
       <c r="A300" t="n">
         <v>323</v>
       </c>
+      <c r="B300" t="n">
+        <v>23.966736</v>
+      </c>
+      <c r="C300" t="n">
+        <v>120.9645109753426</v>
+      </c>
     </row>
     <row r="301">
       <c r="A301" t="n">
         <v>324</v>
       </c>
+      <c r="B301" t="n">
+        <v>23.968544</v>
+      </c>
+      <c r="C301" t="n">
+        <v>120.9620430753427</v>
+      </c>
     </row>
     <row r="302">
       <c r="A302" t="n">
         <v>325</v>
       </c>
+      <c r="B302" t="n">
+        <v>23.96168</v>
+      </c>
+      <c r="C302" t="n">
+        <v>120.9664608753425</v>
+      </c>
     </row>
     <row r="303">
       <c r="A303" t="n">
         <v>326</v>
       </c>
+      <c r="B303" t="n">
+        <v>23.96285</v>
+      </c>
+      <c r="C303" t="n">
+        <v>120.9661060753426</v>
+      </c>
     </row>
     <row r="304">
       <c r="A304" t="n">
         <v>327</v>
       </c>
+      <c r="B304" t="n">
+        <v>23.960842</v>
+      </c>
+      <c r="C304" t="n">
+        <v>120.9689217753424</v>
+      </c>
     </row>
     <row r="305">
       <c r="A305" t="n">
         <v>328</v>
       </c>
+      <c r="B305" t="n">
+        <v>23.963998</v>
+      </c>
+      <c r="C305" t="n">
+        <v>120.9652270753425</v>
+      </c>
     </row>
     <row r="306">
       <c r="A306" t="n">
         <v>329</v>
       </c>
+      <c r="B306" t="n">
+        <v>23.991677</v>
+      </c>
+      <c r="C306" t="n">
+        <v>121.0254677753435</v>
+      </c>
     </row>
     <row r="307">
       <c r="A307" t="n">
         <v>330</v>
       </c>
+      <c r="B307" t="n">
+        <v>23.965805</v>
+      </c>
+      <c r="C307" t="n">
+        <v>120.9699542753426</v>
+      </c>
     </row>
     <row r="308">
       <c r="A308" t="n">
         <v>331</v>
       </c>
+      <c r="B308" t="n">
+        <v>23.978496</v>
+      </c>
+      <c r="C308" t="n">
+        <v>120.989650275343</v>
+      </c>
     </row>
     <row r="309">
       <c r="A309" t="n">
         <v>332</v>
       </c>
+      <c r="B309" t="n">
+        <v>23.967986</v>
+      </c>
+      <c r="C309" t="n">
+        <v>120.9612862753427</v>
+      </c>
     </row>
     <row r="310">
       <c r="A310" t="n">
         <v>333</v>
       </c>
+      <c r="B310" t="n">
+        <v>23.962116</v>
+      </c>
+      <c r="C310" t="n">
+        <v>120.9607376753424</v>
+      </c>
     </row>
     <row r="311">
       <c r="A311" t="n">
         <v>334</v>
       </c>
+      <c r="B311" t="n">
+        <v>23.968445</v>
+      </c>
+      <c r="C311" t="n">
+        <v>120.9719242753426</v>
+      </c>
     </row>
     <row r="312">
       <c r="A312" t="n">
         <v>335</v>
       </c>
+      <c r="B312" t="n">
+        <v>23.96628</v>
+      </c>
+      <c r="C312" t="n">
+        <v>120.9652300753427</v>
+      </c>
     </row>
     <row r="313">
       <c r="A313" t="n">
         <v>336</v>
       </c>
+      <c r="B313" t="n">
+        <v>23.96751</v>
+      </c>
+      <c r="C313" t="n">
+        <v>120.9681083253427</v>
+      </c>
     </row>
     <row r="314">
       <c r="A314" t="n">
         <v>337</v>
       </c>
+      <c r="B314" t="n">
+        <v>23.973408</v>
+      </c>
+      <c r="C314" t="n">
+        <v>120.9698447753428</v>
+      </c>
     </row>
     <row r="315">
       <c r="A315" t="n">
         <v>338</v>
       </c>
+      <c r="B315" t="n">
+        <v>23.970831</v>
+      </c>
+      <c r="C315" t="n">
+        <v>120.9545889753427</v>
+      </c>
     </row>
     <row r="316">
       <c r="A316" t="n">
         <v>339</v>
       </c>
+      <c r="B316" t="n">
+        <v>23.957199</v>
+      </c>
+      <c r="C316" t="n">
+        <v>120.9707391753424</v>
+      </c>
     </row>
     <row r="317">
       <c r="A317" t="n">
         <v>340</v>
       </c>
+      <c r="B317" t="n">
+        <v>23.96385</v>
+      </c>
+      <c r="C317" t="n">
+        <v>120.9663783753425</v>
+      </c>
     </row>
     <row r="318">
       <c r="A318" t="n">
         <v>341</v>
       </c>
+      <c r="B318" t="n">
+        <v>23.96085</v>
+      </c>
+      <c r="C318" t="n">
+        <v>120.9709326753424</v>
+      </c>
     </row>
     <row r="319">
       <c r="A319" t="n">
         <v>342</v>
       </c>
+      <c r="B319" t="n">
+        <v>23.965539</v>
+      </c>
+      <c r="C319" t="n">
+        <v>120.9690739753426</v>
+      </c>
     </row>
     <row r="320">
       <c r="A320" t="n">
         <v>344</v>
       </c>
+      <c r="B320" t="n">
+        <v>23.966045</v>
+      </c>
+      <c r="C320" t="n">
+        <v>120.9310353753427</v>
+      </c>
     </row>
     <row r="321">
       <c r="A321" t="n">
         <v>345</v>
       </c>
+      <c r="B321" t="n">
+        <v>23.94536</v>
+      </c>
+      <c r="C321" t="n">
+        <v>120.952194975342</v>
+      </c>
     </row>
     <row r="322">
       <c r="A322" t="n">
         <v>346</v>
       </c>
+      <c r="B322" t="n">
+        <v>23.97388147</v>
+      </c>
+      <c r="C322" t="n">
+        <v>120.9393102753428</v>
+      </c>
     </row>
     <row r="323">
       <c r="A323" t="n">
         <v>347</v>
       </c>
+      <c r="B323" t="n">
+        <v>23.971102</v>
+      </c>
+      <c r="C323" t="n">
+        <v>120.9724340753428</v>
+      </c>
     </row>
     <row r="324">
       <c r="A324" t="n">
         <v>348</v>
       </c>
+      <c r="B324" t="n">
+        <v>23.9738</v>
+      </c>
+      <c r="C324" t="n">
+        <v>120.9700444753429</v>
+      </c>
     </row>
     <row r="325">
       <c r="A325" t="n">
         <v>349</v>
       </c>
+      <c r="B325" t="n">
+        <v>23.96639</v>
+      </c>
+      <c r="C325" t="n">
+        <v>120.9696819753426</v>
+      </c>
     </row>
     <row r="326">
       <c r="A326" t="n">
         <v>350</v>
       </c>
+      <c r="B326" t="n">
+        <v>23.96414</v>
+      </c>
+      <c r="C326" t="n">
+        <v>120.9634108753425</v>
+      </c>
     </row>
     <row r="327">
       <c r="A327" t="n">
         <v>351</v>
       </c>
+      <c r="B327" t="n">
+        <v>23.97054</v>
+      </c>
+      <c r="C327" t="n">
+        <v>120.9486937753428</v>
+      </c>
     </row>
     <row r="328">
       <c r="A328" t="n">
         <v>352</v>
       </c>
+      <c r="B328" t="n">
+        <v>23.9619043</v>
+      </c>
+      <c r="C328" t="n">
+        <v>120.9683913753423</v>
+      </c>
     </row>
     <row r="329">
       <c r="A329" t="n">
         <v>353</v>
       </c>
+      <c r="B329" t="n">
+        <v>23.964022</v>
+      </c>
+      <c r="C329" t="n">
+        <v>120.9612769753426</v>
+      </c>
     </row>
     <row r="330">
       <c r="A330" t="n">
         <v>354</v>
       </c>
+      <c r="B330" t="n">
+        <v>23.971398</v>
+      </c>
+      <c r="C330" t="n">
+        <v>120.9737560753427</v>
+      </c>
     </row>
     <row r="331">
       <c r="A331" t="n">
         <v>355</v>
       </c>
+      <c r="B331" t="n">
+        <v>23.9690932</v>
+      </c>
+      <c r="C331" t="n">
+        <v>120.9667927753427</v>
+      </c>
     </row>
     <row r="332">
       <c r="A332" t="n">
         <v>356</v>
       </c>
+      <c r="B332" t="n">
+        <v>23.96917</v>
+      </c>
+      <c r="C332" t="n">
+        <v>120.9707454253427</v>
+      </c>
     </row>
     <row r="333">
       <c r="A333" t="n">
         <v>357</v>
       </c>
+      <c r="B333" t="n">
+        <v>23.96674</v>
+      </c>
+      <c r="C333" t="n">
+        <v>120.9644722753427</v>
+      </c>
     </row>
     <row r="334">
       <c r="A334" t="n">
         <v>359</v>
       </c>
+      <c r="B334" t="n">
+        <v>23.964142</v>
+      </c>
+      <c r="C334" t="n">
+        <v>120.9715850753426</v>
+      </c>
     </row>
     <row r="335">
       <c r="A335" t="n">
         <v>360</v>
       </c>
+      <c r="B335" t="n">
+        <v>23.978936</v>
+      </c>
+      <c r="C335" t="n">
+        <v>120.8091339670266</v>
+      </c>
     </row>
     <row r="336">
       <c r="A336" t="n">
         <v>361</v>
       </c>
+      <c r="B336" t="n">
+        <v>23.966807</v>
+      </c>
+      <c r="C336" t="n">
+        <v>120.9690105753426</v>
+      </c>
     </row>
     <row r="337">
       <c r="A337" t="n">
         <v>362</v>
       </c>
+      <c r="B337" t="n">
+        <v>23.96638</v>
+      </c>
+      <c r="C337" t="n">
+        <v>120.9624393753427</v>
+      </c>
     </row>
     <row r="338">
       <c r="A338" t="n">
         <v>363</v>
       </c>
+      <c r="B338" t="n">
+        <v>23.964487</v>
+      </c>
+      <c r="C338" t="n">
+        <v>120.9700220753425</v>
+      </c>
     </row>
     <row r="339">
       <c r="A339" t="n">
         <v>364</v>
       </c>
+      <c r="B339" t="n">
+        <v>23.9645999</v>
+      </c>
+      <c r="C339" t="n">
+        <v>120.9659390753425</v>
+      </c>
     </row>
     <row r="340">
       <c r="A340" t="n">
         <v>365</v>
       </c>
+      <c r="B340" t="n">
+        <v>23.955714</v>
+      </c>
+      <c r="C340" t="n">
+        <v>120.9640885753423</v>
+      </c>
     </row>
     <row r="341">
       <c r="A341" t="n">
         <v>366</v>
       </c>
+      <c r="B341" t="n">
+        <v>23.965174</v>
+      </c>
+      <c r="C341" t="n">
+        <v>120.9626183926774</v>
+      </c>
     </row>
     <row r="342">
       <c r="A342" t="n">
         <v>368</v>
       </c>
+      <c r="B342" t="n">
+        <v>23.96894</v>
+      </c>
+      <c r="C342" t="n">
+        <v>120.9711089753426</v>
+      </c>
     </row>
     <row r="343">
       <c r="A343" t="n">
         <v>369</v>
       </c>
+      <c r="B343" t="n">
+        <v>23.967213</v>
+      </c>
+      <c r="C343" t="n">
+        <v>120.9653001753426</v>
+      </c>
     </row>
     <row r="344">
       <c r="A344" t="n">
         <v>370</v>
       </c>
+      <c r="B344" t="n">
+        <v>23.95644</v>
+      </c>
+      <c r="C344" t="n">
+        <v>120.9798725753423</v>
+      </c>
     </row>
     <row r="345">
       <c r="A345" t="n">
         <v>372</v>
       </c>
+      <c r="B345" t="n">
+        <v>23.96174</v>
+      </c>
+      <c r="C345" t="n">
+        <v>120.9652333753425</v>
+      </c>
     </row>
     <row r="346">
       <c r="A346" t="n">
         <v>373</v>
       </c>
+      <c r="B346" t="n">
+        <v>23.97432</v>
+      </c>
+      <c r="C346" t="n">
+        <v>120.9599478753428</v>
+      </c>
     </row>
     <row r="347">
       <c r="A347" t="n">
         <v>374</v>
       </c>
+      <c r="B347" t="n">
+        <v>23.96267</v>
+      </c>
+      <c r="C347" t="n">
+        <v>120.9656050753425</v>
+      </c>
     </row>
     <row r="348">
       <c r="A348" t="n">
         <v>375</v>
       </c>
+      <c r="B348" t="n">
+        <v>23.962277</v>
+      </c>
+      <c r="C348" t="n">
+        <v>120.9649537753425</v>
+      </c>
     </row>
     <row r="349">
       <c r="A349" t="n">
         <v>376</v>
       </c>
+      <c r="B349" t="n">
+        <v>23.957854</v>
+      </c>
+      <c r="C349" t="n">
+        <v>120.9707625753424</v>
+      </c>
     </row>
     <row r="350">
       <c r="A350" t="n">
         <v>377</v>
       </c>
+      <c r="B350" t="n">
+        <v>23.973124</v>
+      </c>
+      <c r="C350" t="n">
+        <v>120.9650937753429</v>
+      </c>
     </row>
     <row r="351">
       <c r="A351" t="n">
         <v>378</v>
       </c>
+      <c r="B351" t="n">
+        <v>23.965807</v>
+      </c>
+      <c r="C351" t="n">
+        <v>120.9700064753427</v>
+      </c>
     </row>
     <row r="352">
       <c r="A352" t="n">
         <v>379</v>
       </c>
+      <c r="B352" t="n">
+        <v>23.9684655</v>
+      </c>
+      <c r="C352" t="n">
+        <v>120.9676449753427</v>
+      </c>
     </row>
     <row r="353">
       <c r="A353" t="n">
         <v>380</v>
       </c>
+      <c r="B353" t="n">
+        <v>23.97137</v>
+      </c>
+      <c r="C353" t="n">
+        <v>120.9454211753427</v>
+      </c>
     </row>
     <row r="354">
       <c r="A354" t="n">
         <v>381</v>
       </c>
+      <c r="B354" t="n">
+        <v>23.96741</v>
+      </c>
+      <c r="C354" t="n">
+        <v>120.9607962753428</v>
+      </c>
     </row>
     <row r="355">
       <c r="A355" t="n">
         <v>382</v>
       </c>
+      <c r="B355" t="n">
+        <v>23.9665</v>
+      </c>
+      <c r="C355" t="n">
+        <v>120.9602232753426</v>
+      </c>
     </row>
     <row r="356">
       <c r="A356" t="n">
         <v>383</v>
       </c>
+      <c r="B356" t="n">
+        <v>23.96876</v>
+      </c>
+      <c r="C356" t="n">
+        <v>120.9624030753427</v>
+      </c>
     </row>
     <row r="357">
       <c r="A357" t="n">
         <v>384</v>
       </c>
+      <c r="B357" t="n">
+        <v>23.97165</v>
+      </c>
+      <c r="C357" t="n">
+        <v>120.9663022753427</v>
+      </c>
     </row>
     <row r="358">
       <c r="A358" t="n">
         <v>385</v>
       </c>
+      <c r="B358" t="n">
+        <v>23.96151</v>
+      </c>
+      <c r="C358" t="n">
+        <v>120.9670807753426</v>
+      </c>
     </row>
     <row r="359">
       <c r="A359" t="n">
         <v>386</v>
       </c>
+      <c r="B359" t="n">
+        <v>23.96295</v>
+      </c>
+      <c r="C359" t="n">
+        <v>120.9611033753425</v>
+      </c>
     </row>
     <row r="360">
       <c r="A360" t="n">
         <v>387</v>
       </c>
+      <c r="B360" t="n">
+        <v>23.967924</v>
+      </c>
+      <c r="C360" t="n">
+        <v>120.9612455753428</v>
+      </c>
     </row>
     <row r="361">
       <c r="A361" t="n">
         <v>388</v>
       </c>
+      <c r="B361" t="n">
+        <v>23.97132</v>
+      </c>
+      <c r="C361" t="n">
+        <v>120.9457178753428</v>
+      </c>
     </row>
     <row r="362">
       <c r="A362" t="n">
         <v>389</v>
       </c>
+      <c r="B362" t="n">
+        <v>23.9597</v>
+      </c>
+      <c r="C362" t="n">
+        <v>120.9679880753425</v>
+      </c>
     </row>
     <row r="363">
       <c r="A363" t="n">
         <v>390</v>
       </c>
+      <c r="B363" t="n">
+        <v>23.961197</v>
+      </c>
+      <c r="C363" t="n">
+        <v>120.9603478753424</v>
+      </c>
     </row>
     <row r="364">
       <c r="A364" t="n">
         <v>391</v>
       </c>
+      <c r="B364" t="n">
+        <v>23.96536</v>
+      </c>
+      <c r="C364" t="n">
+        <v>120.9754264753427</v>
+      </c>
     </row>
     <row r="365">
       <c r="A365" t="n">
         <v>392</v>
       </c>
+      <c r="B365" t="n">
+        <v>23.97093</v>
+      </c>
+      <c r="C365" t="n">
+        <v>120.9564530753428</v>
+      </c>
     </row>
     <row r="366">
       <c r="A366" t="n">
         <v>393</v>
       </c>
+      <c r="B366" t="n">
+        <v>23.97006</v>
+      </c>
+      <c r="C366" t="n">
+        <v>120.9634314753427</v>
+      </c>
     </row>
     <row r="367">
       <c r="A367" t="n">
         <v>394</v>
       </c>
+      <c r="B367" t="n">
+        <v>23.97399</v>
+      </c>
+      <c r="C367" t="n">
+        <v>120.9477461753429</v>
+      </c>
     </row>
     <row r="368">
       <c r="A368" t="n">
         <v>395</v>
       </c>
+      <c r="B368" t="n">
+        <v>23.97138</v>
+      </c>
+      <c r="C368" t="n">
+        <v>120.9737550753428</v>
+      </c>
     </row>
     <row r="369">
       <c r="A369" t="n">
         <v>396</v>
       </c>
+      <c r="B369" t="n">
+        <v>23.9604721</v>
+      </c>
+      <c r="C369" t="n">
+        <v>120.9697083753424</v>
+      </c>
     </row>
     <row r="370">
       <c r="A370" t="n">
         <v>397</v>
       </c>
+      <c r="B370" t="n">
+        <v>23.973459</v>
+      </c>
+      <c r="C370" t="n">
+        <v>120.9692560753429</v>
+      </c>
     </row>
     <row r="371">
       <c r="A371" t="n">
         <v>398</v>
       </c>
+      <c r="B371" t="n">
+        <v>23.947584</v>
+      </c>
+      <c r="C371" t="n">
+        <v>120.8993490862246</v>
+      </c>
     </row>
     <row r="372">
       <c r="A372" t="n">
         <v>399</v>
       </c>
+      <c r="B372" t="n">
+        <v>23.962417</v>
+      </c>
+      <c r="C372" t="n">
+        <v>120.9646663753426</v>
+      </c>
     </row>
     <row r="373">
       <c r="A373" t="n">
         <v>400</v>
       </c>
+      <c r="B373" t="n">
+        <v>23.962423</v>
+      </c>
+      <c r="C373" t="n">
+        <v>120.9637323753425</v>
+      </c>
     </row>
     <row r="374">
       <c r="A374" t="n">
         <v>401</v>
       </c>
+      <c r="B374" t="n">
+        <v>23.96239</v>
+      </c>
+      <c r="C374" t="n">
+        <v>120.9620736753424</v>
+      </c>
     </row>
     <row r="375">
       <c r="A375" t="n">
         <v>402</v>
       </c>
+      <c r="B375" t="n">
+        <v>23.96723</v>
+      </c>
+      <c r="C375" t="n">
+        <v>120.9702461753425</v>
+      </c>
     </row>
     <row r="376">
       <c r="A376" t="n">
         <v>403</v>
       </c>
+      <c r="B376" t="n">
+        <v>23.967659</v>
+      </c>
+      <c r="C376" t="n">
+        <v>120.9586179753427</v>
+      </c>
     </row>
     <row r="377">
       <c r="A377" t="n">
         <v>404</v>
       </c>
+      <c r="B377" t="n">
+        <v>23.96843</v>
+      </c>
+      <c r="C377" t="n">
+        <v>120.9684647753427</v>
+      </c>
     </row>
     <row r="378">
       <c r="A378" t="n">
         <v>405</v>
       </c>
+      <c r="B378" t="n">
+        <v>23.962033</v>
+      </c>
+      <c r="C378" t="n">
+        <v>120.9680617753425</v>
+      </c>
     </row>
     <row r="379">
       <c r="A379" t="n">
         <v>406</v>
       </c>
+      <c r="B379" t="n">
+        <v>23.966232</v>
+      </c>
+      <c r="C379" t="n">
+        <v>120.9661355753426</v>
+      </c>
     </row>
     <row r="380">
       <c r="A380" t="n">
         <v>408</v>
       </c>
+      <c r="B380" t="n">
+        <v>23.90825</v>
+      </c>
+      <c r="C380" t="n">
+        <v>120.6858242753409</v>
+      </c>
     </row>
     <row r="381">
       <c r="A381" t="n">
         <v>409</v>
       </c>
+      <c r="B381" t="n">
+        <v>23.968406</v>
+      </c>
+      <c r="C381" t="n">
+        <v>120.9559258753427</v>
+      </c>
     </row>
     <row r="382">
       <c r="A382" t="n">
         <v>410</v>
       </c>
+      <c r="B382" t="n">
+        <v>23.96059</v>
+      </c>
+      <c r="C382" t="n">
+        <v>120.9968626753425</v>
+      </c>
     </row>
     <row r="383">
       <c r="A383" t="n">
         <v>411</v>
       </c>
+      <c r="B383" t="n">
+        <v>23.95456</v>
+      </c>
+      <c r="C383" t="n">
+        <v>120.9763642753422</v>
+      </c>
     </row>
     <row r="384">
       <c r="A384" t="n">
         <v>412</v>
       </c>
+      <c r="B384" t="n">
+        <v>23.96604</v>
+      </c>
+      <c r="C384" t="n">
+        <v>120.9597709753427</v>
+      </c>
     </row>
     <row r="385">
       <c r="A385" t="n">
         <v>413</v>
       </c>
+      <c r="B385" t="n">
+        <v>23.966948</v>
+      </c>
+      <c r="C385" t="n">
+        <v>120.9614316753427</v>
+      </c>
     </row>
     <row r="386">
       <c r="A386" t="n">
         <v>414</v>
       </c>
+      <c r="B386" t="n">
+        <v>23.967328</v>
+      </c>
+      <c r="C386" t="n">
+        <v>120.9651605753426</v>
+      </c>
     </row>
     <row r="387">
       <c r="A387" t="n">
         <v>415</v>
       </c>
+      <c r="B387" t="n">
+        <v>23.964477</v>
+      </c>
+      <c r="C387" t="n">
+        <v>120.9695419753426</v>
+      </c>
     </row>
     <row r="388">
       <c r="A388" t="n">
         <v>416</v>
       </c>
+      <c r="B388" t="n">
+        <v>23.96445</v>
+      </c>
+      <c r="C388" t="n">
+        <v>120.9694934753427</v>
+      </c>
     </row>
     <row r="389">
       <c r="A389" t="n">
         <v>417</v>
       </c>
+      <c r="B389" t="n">
+        <v>23.967569</v>
+      </c>
+      <c r="C389" t="n">
+        <v>120.9600852753426</v>
+      </c>
     </row>
     <row r="390">
       <c r="A390" t="n">
         <v>418</v>
       </c>
+      <c r="B390" t="n">
+        <v>23.9628202</v>
+      </c>
+      <c r="C390" t="n">
+        <v>120.9671274753425</v>
+      </c>
     </row>
     <row r="391">
       <c r="A391" t="n">
         <v>419</v>
       </c>
+      <c r="B391" t="n">
+        <v>23.963984</v>
+      </c>
+      <c r="C391" t="n">
+        <v>120.9635888753426</v>
+      </c>
     </row>
     <row r="392">
       <c r="A392" t="n">
         <v>420</v>
       </c>
+      <c r="B392" t="n">
+        <v>23.96254</v>
+      </c>
+      <c r="C392" t="n">
+        <v>120.9625431753425</v>
+      </c>
     </row>
     <row r="393">
       <c r="A393" t="n">
         <v>421</v>
       </c>
+      <c r="B393" t="n">
+        <v>23.9708693</v>
+      </c>
+      <c r="C393" t="n">
+        <v>120.9642007753427</v>
+      </c>
     </row>
     <row r="394">
       <c r="A394" t="n">
         <v>422</v>
       </c>
+      <c r="B394" t="n">
+        <v>23.9656</v>
+      </c>
+      <c r="C394" t="n">
+        <v>120.9656265753425</v>
+      </c>
     </row>
     <row r="395">
       <c r="A395" t="n">
         <v>423</v>
       </c>
+      <c r="B395" t="n">
+        <v>23.96092</v>
+      </c>
+      <c r="C395" t="n">
+        <v>120.9656403753425</v>
+      </c>
     </row>
     <row r="396">
       <c r="A396" t="n">
         <v>424</v>
       </c>
+      <c r="B396" t="n">
+        <v>23.96766</v>
+      </c>
+      <c r="C396" t="n">
+        <v>120.9584476753427</v>
+      </c>
     </row>
     <row r="397">
       <c r="A397" t="n">
         <v>425</v>
       </c>
+      <c r="B397" t="n">
+        <v>23.9676485</v>
+      </c>
+      <c r="C397" t="n">
+        <v>120.9585227753427</v>
+      </c>
     </row>
     <row r="398">
       <c r="A398" t="n">
         <v>426</v>
       </c>
+      <c r="B398" t="n">
+        <v>23.968</v>
+      </c>
+      <c r="C398" t="n">
+        <v>120.9490880753426</v>
+      </c>
     </row>
     <row r="399">
       <c r="A399" t="n">
         <v>427</v>
       </c>
+      <c r="B399" t="n">
+        <v>23.97182</v>
+      </c>
+      <c r="C399" t="n">
+        <v>120.9560862753429</v>
+      </c>
     </row>
     <row r="400">
       <c r="A400" t="n">
         <v>428</v>
       </c>
+      <c r="B400" t="n">
+        <v>23.964508</v>
+      </c>
+      <c r="C400" t="n">
+        <v>120.9638144753426</v>
+      </c>
     </row>
     <row r="401">
       <c r="A401" t="n">
         <v>429</v>
       </c>
+      <c r="B401" t="n">
+        <v>23.962233</v>
+      </c>
+      <c r="C401" t="n">
+        <v>120.9613081753424</v>
+      </c>
     </row>
     <row r="402">
       <c r="A402" t="n">
         <v>430</v>
       </c>
+      <c r="B402" t="n">
+        <v>23.9674258</v>
+      </c>
+      <c r="C402" t="n">
+        <v>120.9675710753427</v>
+      </c>
     </row>
     <row r="403">
       <c r="A403" t="n">
         <v>431</v>
       </c>
+      <c r="B403" t="n">
+        <v>23.97766</v>
+      </c>
+      <c r="C403" t="n">
+        <v>120.987404975343</v>
+      </c>
     </row>
     <row r="404">
       <c r="A404" t="n">
         <v>432</v>
       </c>
+      <c r="B404" t="n">
+        <v>23.97059</v>
+      </c>
+      <c r="C404" t="n">
+        <v>120.9530473753427</v>
+      </c>
     </row>
     <row r="405">
       <c r="A405" t="n">
         <v>433</v>
       </c>
+      <c r="B405" t="n">
+        <v>23.96883</v>
+      </c>
+      <c r="C405" t="n">
+        <v>120.9577192753427</v>
+      </c>
     </row>
     <row r="406">
       <c r="A406" t="n">
         <v>434</v>
       </c>
+      <c r="B406" t="n">
+        <v>23.970823</v>
+      </c>
+      <c r="C406" t="n">
+        <v>120.9474666753427</v>
+      </c>
     </row>
     <row r="407">
       <c r="A407" t="n">
         <v>435</v>
       </c>
+      <c r="B407" t="n">
+        <v>23.978936</v>
+      </c>
+      <c r="C407" t="n">
+        <v>120.8091339670266</v>
+      </c>
     </row>
     <row r="408">
       <c r="A408" t="n">
         <v>436</v>
       </c>
+      <c r="B408" t="n">
+        <v>23.97089</v>
+      </c>
+      <c r="C408" t="n">
+        <v>120.9656892753428</v>
+      </c>
     </row>
     <row r="409">
       <c r="A409" t="n">
         <v>437</v>
       </c>
+      <c r="B409" t="n">
+        <v>23.96387</v>
+      </c>
+      <c r="C409" t="n">
+        <v>120.9634836753425</v>
+      </c>
     </row>
     <row r="410">
       <c r="A410" t="n">
         <v>438</v>
       </c>
+      <c r="B410" t="n">
+        <v>23.966992</v>
+      </c>
+      <c r="C410" t="n">
+        <v>120.9626135753427</v>
+      </c>
     </row>
     <row r="411">
       <c r="A411" t="n">
         <v>439</v>
       </c>
+      <c r="B411" t="n">
+        <v>23.96521</v>
+      </c>
+      <c r="C411" t="n">
+        <v>120.9627420753425</v>
+      </c>
     </row>
     <row r="412">
       <c r="A412" t="n">
         <v>440</v>
       </c>
+      <c r="B412" t="n">
+        <v>23.9682396</v>
+      </c>
+      <c r="C412" t="n">
+        <v>120.9679978753426</v>
+      </c>
     </row>
     <row r="413">
       <c r="A413" t="n">
         <v>441</v>
       </c>
+      <c r="B413" t="n">
+        <v>23.96448</v>
+      </c>
+      <c r="C413" t="n">
+        <v>120.9624336753425</v>
+      </c>
     </row>
     <row r="414">
       <c r="A414" t="n">
         <v>442</v>
       </c>
+      <c r="B414" t="n">
+        <v>23.96879997</v>
+      </c>
+      <c r="C414" t="n">
+        <v>120.9709941753426</v>
+      </c>
     </row>
     <row r="415">
       <c r="A415" t="n">
@@ -3752,36 +4994,78 @@
       <c r="A416" t="n">
         <v>444</v>
       </c>
+      <c r="B416" t="n">
+        <v>23.961047</v>
+      </c>
+      <c r="C416" t="n">
+        <v>120.9657795753425</v>
+      </c>
     </row>
     <row r="417">
       <c r="A417" t="n">
         <v>445</v>
       </c>
+      <c r="B417" t="n">
+        <v>23.97135</v>
+      </c>
+      <c r="C417" t="n">
+        <v>120.9666005753428</v>
+      </c>
     </row>
     <row r="418">
       <c r="A418" t="n">
         <v>446</v>
       </c>
+      <c r="B418" t="n">
+        <v>23.96788</v>
+      </c>
+      <c r="C418" t="n">
+        <v>120.9612394753427</v>
+      </c>
     </row>
     <row r="419">
       <c r="A419" t="n">
         <v>447</v>
       </c>
+      <c r="B419" t="n">
+        <v>23.96272</v>
+      </c>
+      <c r="C419" t="n">
+        <v>120.9629192753425</v>
+      </c>
     </row>
     <row r="420">
       <c r="A420" t="n">
         <v>448</v>
       </c>
+      <c r="B420" t="n">
+        <v>23.97138</v>
+      </c>
+      <c r="C420" t="n">
+        <v>120.9667191753427</v>
+      </c>
     </row>
     <row r="421">
       <c r="A421" t="n">
         <v>449</v>
       </c>
+      <c r="B421" t="n">
+        <v>23.96744</v>
+      </c>
+      <c r="C421" t="n">
+        <v>120.9595961753426</v>
+      </c>
     </row>
     <row r="422">
       <c r="A422" t="n">
         <v>450</v>
       </c>
+      <c r="B422" t="n">
+        <v>23.96739</v>
+      </c>
+      <c r="C422" t="n">
+        <v>120.9607971753426</v>
+      </c>
     </row>
     <row r="423">
       <c r="A423" t="n">
@@ -3792,46 +5076,100 @@
       <c r="A424" t="n">
         <v>452</v>
       </c>
+      <c r="B424" t="n">
+        <v>23.967452</v>
+      </c>
+      <c r="C424" t="n">
+        <v>120.9517203753427</v>
+      </c>
     </row>
     <row r="425">
       <c r="A425" t="n">
         <v>454</v>
       </c>
+      <c r="B425" t="n">
+        <v>23.96207</v>
+      </c>
+      <c r="C425" t="n">
+        <v>120.9651801753425</v>
+      </c>
     </row>
     <row r="426">
       <c r="A426" t="n">
         <v>455</v>
       </c>
+      <c r="B426" t="n">
+        <v>23.9693977</v>
+      </c>
+      <c r="C426" t="n">
+        <v>120.9613704753427</v>
+      </c>
     </row>
     <row r="427">
       <c r="A427" t="n">
         <v>456</v>
       </c>
+      <c r="B427" t="n">
+        <v>23.9624294</v>
+      </c>
+      <c r="C427" t="n">
+        <v>120.9599276753425</v>
+      </c>
     </row>
     <row r="428">
       <c r="A428" t="n">
         <v>457</v>
       </c>
+      <c r="B428" t="n">
+        <v>23.96291</v>
+      </c>
+      <c r="C428" t="n">
+        <v>120.9659205753425</v>
+      </c>
     </row>
     <row r="429">
       <c r="A429" t="n">
         <v>458</v>
       </c>
+      <c r="B429" t="n">
+        <v>23.96766</v>
+      </c>
+      <c r="C429" t="n">
+        <v>120.9680084753426</v>
+      </c>
     </row>
     <row r="430">
       <c r="A430" t="n">
         <v>459</v>
       </c>
+      <c r="B430" t="n">
+        <v>23.971466</v>
+      </c>
+      <c r="C430" t="n">
+        <v>120.9563388753427</v>
+      </c>
     </row>
     <row r="431">
       <c r="A431" t="n">
         <v>460</v>
       </c>
+      <c r="B431" t="n">
+        <v>23.965049</v>
+      </c>
+      <c r="C431" t="n">
+        <v>120.9742859753425</v>
+      </c>
     </row>
     <row r="432">
       <c r="A432" t="n">
         <v>461</v>
       </c>
+      <c r="B432" t="n">
+        <v>23.9628488</v>
+      </c>
+      <c r="C432" t="n">
+        <v>120.9617298753425</v>
+      </c>
     </row>
     <row r="433">
       <c r="A433" t="n">
@@ -3842,180 +5180,396 @@
       <c r="A434" t="n">
         <v>463</v>
       </c>
+      <c r="B434" t="n">
+        <v>23.973062</v>
+      </c>
+      <c r="C434" t="n">
+        <v>120.9721478753429</v>
+      </c>
     </row>
     <row r="435">
       <c r="A435" t="n">
         <v>464</v>
       </c>
+      <c r="B435" t="n">
+        <v>23.966953</v>
+      </c>
+      <c r="C435" t="n">
+        <v>120.9665717426772</v>
+      </c>
     </row>
     <row r="436">
       <c r="A436" t="n">
         <v>465</v>
       </c>
+      <c r="B436" t="n">
+        <v>23.962512</v>
+      </c>
+      <c r="C436" t="n">
+        <v>120.9676935753425</v>
+      </c>
     </row>
     <row r="437">
       <c r="A437" t="n">
         <v>466</v>
       </c>
+      <c r="B437" t="n">
+        <v>23.962277</v>
+      </c>
+      <c r="C437" t="n">
+        <v>120.9649537753425</v>
+      </c>
     </row>
     <row r="438">
       <c r="A438" t="n">
         <v>467</v>
       </c>
+      <c r="B438" t="n">
+        <v>23.9669</v>
+      </c>
+      <c r="C438" t="n">
+        <v>120.9613448753426</v>
+      </c>
     </row>
     <row r="439">
       <c r="A439" t="n">
         <v>468</v>
       </c>
+      <c r="B439" t="n">
+        <v>23.96461</v>
+      </c>
+      <c r="C439" t="n">
+        <v>120.9681389753425</v>
+      </c>
     </row>
     <row r="440">
       <c r="A440" t="n">
         <v>469</v>
       </c>
+      <c r="B440" t="n">
+        <v>23.9623</v>
+      </c>
+      <c r="C440" t="n">
+        <v>120.9647318753425</v>
+      </c>
     </row>
     <row r="441">
       <c r="A441" t="n">
         <v>470</v>
       </c>
+      <c r="B441" t="n">
+        <v>23.96207</v>
+      </c>
+      <c r="C441" t="n">
+        <v>120.9669525753426</v>
+      </c>
     </row>
     <row r="442">
       <c r="A442" t="n">
         <v>472</v>
       </c>
+      <c r="B442" t="n">
+        <v>23.97152977</v>
+      </c>
+      <c r="C442" t="n">
+        <v>120.9610602753428</v>
+      </c>
     </row>
     <row r="443">
       <c r="A443" t="n">
         <v>473</v>
       </c>
+      <c r="B443" t="n">
+        <v>23.967266</v>
+      </c>
+      <c r="C443" t="n">
+        <v>120.9673060753425</v>
+      </c>
     </row>
     <row r="444">
       <c r="A444" t="n">
         <v>474</v>
       </c>
+      <c r="B444" t="n">
+        <v>23.962156</v>
+      </c>
+      <c r="C444" t="n">
+        <v>120.9670519753424</v>
+      </c>
     </row>
     <row r="445">
       <c r="A445" t="n">
         <v>475</v>
       </c>
+      <c r="B445" t="n">
+        <v>23.967208</v>
+      </c>
+      <c r="C445" t="n">
+        <v>120.9685393753426</v>
+      </c>
     </row>
     <row r="446">
       <c r="A446" t="n">
         <v>476</v>
       </c>
+      <c r="B446" t="n">
+        <v>23.971742</v>
+      </c>
+      <c r="C446" t="n">
+        <v>120.9609790753428</v>
+      </c>
     </row>
     <row r="447">
       <c r="A447" t="n">
         <v>477</v>
       </c>
+      <c r="B447" t="n">
+        <v>23.962997</v>
+      </c>
+      <c r="C447" t="n">
+        <v>120.9662738753426</v>
+      </c>
     </row>
     <row r="448">
       <c r="A448" t="n">
         <v>478</v>
       </c>
+      <c r="B448" t="n">
+        <v>23.96781</v>
+      </c>
+      <c r="C448" t="n">
+        <v>120.9582961753426</v>
+      </c>
     </row>
     <row r="449">
       <c r="A449" t="n">
         <v>479</v>
       </c>
+      <c r="B449" t="n">
+        <v>23.965665</v>
+      </c>
+      <c r="C449" t="n">
+        <v>120.9701977753425</v>
+      </c>
     </row>
     <row r="450">
       <c r="A450" t="n">
         <v>480</v>
       </c>
+      <c r="B450" t="n">
+        <v>23.96813</v>
+      </c>
+      <c r="C450" t="n">
+        <v>120.9580218753427</v>
+      </c>
     </row>
     <row r="451">
       <c r="A451" t="n">
         <v>481</v>
       </c>
+      <c r="B451" t="n">
+        <v>23.97192</v>
+      </c>
+      <c r="C451" t="n">
+        <v>120.9747171753427</v>
+      </c>
     </row>
     <row r="452">
       <c r="A452" t="n">
         <v>482</v>
       </c>
+      <c r="B452" t="n">
+        <v>23.96966</v>
+      </c>
+      <c r="C452" t="n">
+        <v>120.9663247753426</v>
+      </c>
     </row>
     <row r="453">
       <c r="A453" t="n">
         <v>483</v>
       </c>
+      <c r="B453" t="n">
+        <v>23.9665924</v>
+      </c>
+      <c r="C453" t="n">
+        <v>120.9552095753426</v>
+      </c>
     </row>
     <row r="454">
       <c r="A454" t="n">
         <v>484</v>
       </c>
+      <c r="B454" t="n">
+        <v>23.962277</v>
+      </c>
+      <c r="C454" t="n">
+        <v>120.9649537753425</v>
+      </c>
     </row>
     <row r="455">
       <c r="A455" t="n">
         <v>485</v>
       </c>
+      <c r="B455" t="n">
+        <v>23.964194</v>
+      </c>
+      <c r="C455" t="n">
+        <v>120.9610920753427</v>
+      </c>
     </row>
     <row r="456">
       <c r="A456" t="n">
         <v>486</v>
       </c>
+      <c r="B456" t="n">
+        <v>23.96733</v>
+      </c>
+      <c r="C456" t="n">
+        <v>120.9598856753427</v>
+      </c>
     </row>
     <row r="457">
       <c r="A457" t="n">
         <v>487</v>
       </c>
+      <c r="B457" t="n">
+        <v>23.96974</v>
+      </c>
+      <c r="C457" t="n">
+        <v>120.9505780753426</v>
+      </c>
     </row>
     <row r="458">
       <c r="A458" t="n">
         <v>488</v>
       </c>
+      <c r="B458" t="n">
+        <v>23.96736</v>
+      </c>
+      <c r="C458" t="n">
+        <v>120.9626755753426</v>
+      </c>
     </row>
     <row r="459">
       <c r="A459" t="n">
         <v>489</v>
       </c>
+      <c r="B459" t="n">
+        <v>23.967163</v>
+      </c>
+      <c r="C459" t="n">
+        <v>120.9685677753427</v>
+      </c>
     </row>
     <row r="460">
       <c r="A460" t="n">
         <v>490</v>
       </c>
+      <c r="B460" t="n">
+        <v>23.9668697</v>
+      </c>
+      <c r="C460" t="n">
+        <v>120.9646365753426</v>
+      </c>
     </row>
     <row r="461">
       <c r="A461" t="n">
         <v>491</v>
       </c>
+      <c r="B461" t="n">
+        <v>23.968897</v>
+      </c>
+      <c r="C461" t="n">
+        <v>120.9538380753427</v>
+      </c>
     </row>
     <row r="462">
       <c r="A462" t="n">
         <v>492</v>
       </c>
+      <c r="B462" t="n">
+        <v>23.960222</v>
+      </c>
+      <c r="C462" t="n">
+        <v>120.9745794753423</v>
+      </c>
     </row>
     <row r="463">
       <c r="A463" t="n">
         <v>493</v>
       </c>
+      <c r="B463" t="n">
+        <v>23.97145</v>
+      </c>
+      <c r="C463" t="n">
+        <v>120.9647044753429</v>
+      </c>
     </row>
     <row r="464">
       <c r="A464" t="n">
         <v>494</v>
       </c>
+      <c r="B464" t="n">
+        <v>23.970723</v>
+      </c>
+      <c r="C464" t="n">
+        <v>120.9668408753427</v>
+      </c>
     </row>
     <row r="465">
       <c r="A465" t="n">
         <v>495</v>
       </c>
+      <c r="B465" t="n">
+        <v>23.96468</v>
+      </c>
+      <c r="C465" t="n">
+        <v>120.9678260753425</v>
+      </c>
     </row>
     <row r="466">
       <c r="A466" t="n">
         <v>496</v>
       </c>
+      <c r="B466" t="n">
+        <v>23.96884</v>
+      </c>
+      <c r="C466" t="n">
+        <v>120.9615968753427</v>
+      </c>
     </row>
     <row r="467">
       <c r="A467" t="n">
         <v>497</v>
       </c>
+      <c r="B467" t="n">
+        <v>23.96685</v>
+      </c>
+      <c r="C467" t="n">
+        <v>120.9714073753428</v>
+      </c>
     </row>
     <row r="468">
       <c r="A468" t="n">
         <v>498</v>
       </c>
+      <c r="B468" t="n">
+        <v>23.97065</v>
+      </c>
+      <c r="C468" t="n">
+        <v>120.9480974753427</v>
+      </c>
     </row>
     <row r="469">
       <c r="A469" t="n">
         <v>499</v>
+      </c>
+      <c r="B469" t="n">
+        <v>23.96683</v>
+      </c>
+      <c r="C469" t="n">
+        <v>120.9601715753426</v>
       </c>
     </row>
     <row r="470">

</xml_diff>